<commit_message>
Last day of SURE. Wrote code to check if all flux for a reaction were positive or negative.
</commit_message>
<xml_diff>
--- a/matlab/MeCorr/VariablesSaved/analysis.xlsx
+++ b/matlab/MeCorr/VariablesSaved/analysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laure\Documents\CancerMetabRes\egem-lf\matlab\MeCorr\VariablesSaved\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED3BA40A-30B4-44EE-9733-30D7DF0BBA47}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A97A4029-A9C8-419E-A639-ED05CFF3477E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-75" yWindow="570" windowWidth="10350" windowHeight="7875" firstSheet="1" activeTab="1" xr2:uid="{41914AB9-F57C-4F6C-9BD0-256246B50507}"/>
+    <workbookView xWindow="-75" yWindow="570" windowWidth="10350" windowHeight="7875" xr2:uid="{41914AB9-F57C-4F6C-9BD0-256246B50507}"/>
   </bookViews>
   <sheets>
     <sheet name="Expected" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="123">
   <si>
     <t>Reaction contributes to methylation</t>
   </si>
@@ -314,9 +314,6 @@
     <t>only 3</t>
   </si>
   <si>
-    <t>cmp+dadp&lt;=&gt;cdp+dadp (all cytosol)</t>
-  </si>
-  <si>
     <t>form nmn</t>
   </si>
   <si>
@@ -423,12 +420,6 @@
     <t>int34: ASNt4, CYTK13</t>
   </si>
   <si>
-    <t>phosphorylate pail45p_hs in cytosol</t>
-  </si>
-  <si>
-    <t>phosphorylate pail45p_hs in nucleus</t>
-  </si>
-  <si>
     <t>The Direct Interaction Between ASH2, a Drosophila Trithorax Group Protein, and SKTL, a Nuclear Phosphatidylinositol 4-Phosphate 5-Kinase, Implies a Role for Phosphatidylinositol 4,5-Bisphosphate in Maintaining Transcriptionally Active Chromatin</t>
   </si>
   <si>
@@ -438,7 +429,25 @@
     <t>PIP2 may be a part of rDNA silencing complex</t>
   </si>
   <si>
-    <t>Educated Guess</t>
+    <t>Reaction Description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">forward: c-&gt;n, reversible </t>
+  </si>
+  <si>
+    <t>cmp+dadp&lt;=&gt;cdp+dadp (all c)</t>
+  </si>
+  <si>
+    <t>phosphorylate pail45p_hs -&gt; pail345p_hs (all c)</t>
+  </si>
+  <si>
+    <t>phosphorylate pail4p_hs -&gt; pail45p_hs (all n)</t>
+  </si>
+  <si>
+    <t>Signaling</t>
+  </si>
+  <si>
+    <t>PI4P5K</t>
   </si>
 </sst>
 </file>
@@ -834,8 +843,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14F01ED5-8303-49E5-8541-1CF09681FF65}">
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1022,10 +1031,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F39EF18E-5253-4B54-A7C9-839494E6B72D}">
-  <dimension ref="A1:K35"/>
+  <dimension ref="A1:K34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="82" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView topLeftCell="A3" zoomScale="82" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27:A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1033,8 +1042,8 @@
     <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="30.7109375" customWidth="1"/>
-    <col min="4" max="4" width="13" style="4" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="4"/>
+    <col min="4" max="4" width="6.85546875" style="4" customWidth="1"/>
+    <col min="5" max="5" width="23.7109375" style="4" customWidth="1"/>
     <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16.85546875" customWidth="1"/>
     <col min="8" max="9" width="9.140625" style="4"/>
@@ -1157,7 +1166,7 @@
         <v>1</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F4" t="s">
         <v>65</v>
@@ -1189,11 +1198,11 @@
       <c r="C5" t="s">
         <v>31</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="6">
         <v>1</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>73</v>
+        <v>117</v>
       </c>
       <c r="F5" t="s">
         <v>64</v>
@@ -1292,7 +1301,7 @@
         <v>1</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>78</v>
+        <v>118</v>
       </c>
       <c r="F8" t="s">
         <v>64</v>
@@ -1354,11 +1363,11 @@
       <c r="C10" t="s">
         <v>39</v>
       </c>
-      <c r="D10" s="4">
-        <v>1</v>
+      <c r="D10" s="6">
+        <v>-1</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="F10" t="s">
         <v>64</v>
@@ -1371,10 +1380,13 @@
       </c>
       <c r="I10" s="4">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="J10">
         <v>-0.3192374743410385</v>
+      </c>
+      <c r="K10" s="4">
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -1391,7 +1403,7 @@
         <v>1</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F11" t="s">
         <v>65</v>
@@ -1487,7 +1499,7 @@
         <v>1</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="F14" t="s">
         <v>64</v>
@@ -1649,7 +1661,7 @@
         <v>1</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F19" t="s">
         <v>64</v>
@@ -1814,59 +1826,65 @@
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C25" s="1" t="s">
         <v>81</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C26" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="C27" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="C28" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>86</v>
+        <v>87</v>
+      </c>
+      <c r="C29" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>87</v>
+        <v>88</v>
+      </c>
+      <c r="C30" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>88</v>
+      <c r="A31" s="1" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>89</v>
+        <v>122</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
-        <v>119</v>
+      <c r="A33" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -1875,11 +1893,6 @@
       </c>
       <c r="C34" t="s">
         <v>34</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -1889,243 +1902,276 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D0304A2-389C-497F-9879-0B26FAB612FF}">
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.85546875" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" customWidth="1"/>
-    <col min="11" max="11" width="30.5703125" customWidth="1"/>
+    <col min="2" max="2" width="20.28515625" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" customWidth="1"/>
+    <col min="4" max="4" width="5.5703125" customWidth="1"/>
+    <col min="5" max="5" width="5.85546875" customWidth="1"/>
+    <col min="6" max="6" width="5.7109375" customWidth="1"/>
+    <col min="7" max="7" width="5.140625" customWidth="1"/>
+    <col min="8" max="8" width="5.7109375" customWidth="1"/>
+    <col min="9" max="9" width="4.42578125" customWidth="1"/>
+    <col min="12" max="12" width="30.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C1" t="s">
         <v>100</v>
       </c>
-      <c r="B1" t="s">
-        <v>101</v>
-      </c>
-      <c r="C1" t="s">
-        <v>107</v>
-      </c>
       <c r="D1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E1" t="s">
         <v>109</v>
       </c>
       <c r="F1" t="s">
-        <v>81</v>
+        <v>108</v>
       </c>
       <c r="G1" t="s">
-        <v>108</v>
+        <v>80</v>
       </c>
       <c r="H1" t="s">
+        <v>107</v>
+      </c>
+      <c r="I1" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D2" t="s">
+        <v>104</v>
+      </c>
+      <c r="E2" s="6"/>
+      <c r="F2">
+        <v>-1</v>
+      </c>
+      <c r="G2">
+        <f>E2*F2</f>
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>93</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C3" t="s">
         <v>103</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D3" t="s">
+        <v>104</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>-1</v>
+      </c>
+      <c r="G3">
+        <f t="shared" ref="G3:G8" si="0">E3*F3</f>
+        <v>-1</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>94</v>
+      </c>
+      <c r="B4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" t="s">
+        <v>101</v>
+      </c>
+      <c r="D4" t="s">
         <v>105</v>
       </c>
-      <c r="D2" s="6"/>
-      <c r="E2">
-        <v>-1</v>
-      </c>
-      <c r="F2">
-        <f>D2*E2</f>
+      <c r="E4">
+        <v>-1</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="H4">
+        <v>-1</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>95</v>
+      </c>
+      <c r="B5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" t="s">
+        <v>102</v>
+      </c>
+      <c r="D5" t="s">
+        <v>104</v>
+      </c>
+      <c r="E5" s="6"/>
+      <c r="F5">
+        <v>-1</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>94</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="H5">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>96</v>
+      </c>
+      <c r="B6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" t="s">
+        <v>103</v>
+      </c>
+      <c r="D6" t="s">
         <v>104</v>
       </c>
-      <c r="C3" t="s">
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>-1</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="H6">
+        <v>-1</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>97</v>
+      </c>
+      <c r="B7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" t="s">
+        <v>101</v>
+      </c>
+      <c r="D7" t="s">
         <v>105</v>
       </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3">
-        <v>-1</v>
-      </c>
-      <c r="F3">
-        <f t="shared" ref="F3:F8" si="0">D3*E3</f>
-        <v>-1</v>
-      </c>
-      <c r="G3">
-        <v>1</v>
-      </c>
-      <c r="H3">
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <v>-1</v>
+      </c>
+      <c r="I7">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>95</v>
-      </c>
-      <c r="B4" t="s">
-        <v>102</v>
-      </c>
-      <c r="C4" t="s">
-        <v>106</v>
-      </c>
-      <c r="D4">
-        <v>-1</v>
-      </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-      <c r="F4">
-        <f t="shared" si="0"/>
-        <v>-1</v>
-      </c>
-      <c r="G4">
-        <v>-1</v>
-      </c>
-      <c r="H4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>96</v>
-      </c>
-      <c r="B5" t="s">
-        <v>103</v>
-      </c>
-      <c r="C5" t="s">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>98</v>
+      </c>
+      <c r="B8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" t="s">
+        <v>101</v>
+      </c>
+      <c r="D8" t="s">
         <v>105</v>
       </c>
-      <c r="D5" s="6"/>
-      <c r="E5">
-        <v>-1</v>
-      </c>
-      <c r="F5">
-        <f t="shared" si="0"/>
+      <c r="E8" s="6">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H8">
+        <v>-1</v>
+      </c>
+      <c r="I8">
         <v>0</v>
       </c>
-      <c r="G5">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>97</v>
-      </c>
-      <c r="B6" t="s">
-        <v>104</v>
-      </c>
-      <c r="C6" t="s">
-        <v>105</v>
-      </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
-      <c r="E6">
-        <v>-1</v>
-      </c>
-      <c r="F6">
-        <f t="shared" si="0"/>
-        <v>-1</v>
-      </c>
-      <c r="G6">
-        <v>-1</v>
-      </c>
-      <c r="H6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>98</v>
-      </c>
-      <c r="B7" t="s">
-        <v>102</v>
-      </c>
-      <c r="C7" t="s">
-        <v>106</v>
-      </c>
-      <c r="D7">
-        <v>1</v>
-      </c>
-      <c r="E7">
-        <v>1</v>
-      </c>
-      <c r="F7">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="G7">
-        <v>-1</v>
-      </c>
-      <c r="H7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>99</v>
-      </c>
-      <c r="B8" t="s">
-        <v>102</v>
-      </c>
-      <c r="C8" t="s">
-        <v>106</v>
-      </c>
-      <c r="D8" s="6">
-        <v>1</v>
-      </c>
-      <c r="E8">
-        <v>1</v>
-      </c>
-      <c r="F8">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="G8">
-        <v>-1</v>
-      </c>
-      <c r="H8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="255" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:9" ht="255" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="240" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="B12" s="5"/>
+      <c r="C12" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>112</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="240" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="B12" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>113</v>
       </c>
     </row>
   </sheetData>

</xml_diff>